<commit_message>
alternate product for deprecated filter
</commit_message>
<xml_diff>
--- a/ciclops-core/BOM.xlsx
+++ b/ciclops-core/BOM.xlsx
@@ -574,9 +574,6 @@
     <t>Optical fiber patchcord</t>
   </si>
   <si>
-    <t>504/12m</t>
-  </si>
-  <si>
     <t>Semrock</t>
   </si>
   <si>
@@ -593,9 +590,6 @@
   </si>
   <si>
     <t>epoxy to attach PMT onto shutter</t>
-  </si>
-  <si>
-    <t>504/12 nm emission filter</t>
   </si>
   <si>
     <t>RC0603JR-0716KL</t>
@@ -728,6 +722,12 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>FF01-515/30</t>
+  </si>
+  <si>
+    <t>515/30 nm emission filter</t>
   </si>
 </sst>
 </file>
@@ -1295,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="35" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1421,13 +1421,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17">
@@ -1581,7 +1581,7 @@
         <v>171</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
@@ -1619,13 +1619,13 @@
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>229</v>
-      </c>
       <c r="D9" s="27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="28"/>
@@ -1663,13 +1663,13 @@
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="27" t="s">
         <v>228</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>230</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
@@ -1712,7 +1712,7 @@
       <c r="C11" s="26"/>
       <c r="D11" s="27"/>
       <c r="E11" s="32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28">
@@ -1883,16 +1883,16 @@
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28">
@@ -1929,16 +1929,16 @@
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C16" s="26">
         <v>61300211121</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17">
@@ -1975,16 +1975,16 @@
     <row r="17" spans="1:26" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C17" s="26">
         <v>61300311121</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17">
@@ -2021,16 +2021,16 @@
     <row r="18" spans="1:26" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>216</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>218</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17">
@@ -2208,13 +2208,13 @@
         <v>31</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>195</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17">
@@ -2254,13 +2254,13 @@
         <v>31</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D23" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>194</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>196</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17">
@@ -2300,13 +2300,13 @@
         <v>31</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17">
@@ -2346,13 +2346,13 @@
         <v>31</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17">
@@ -2392,13 +2392,13 @@
         <v>31</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17">
@@ -2435,16 +2435,16 @@
     <row r="27" spans="1:26" ht="15" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17">
@@ -2757,16 +2757,16 @@
     <row r="34" spans="1:26" ht="15" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>52</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="17">
@@ -3290,7 +3290,7 @@
         <v>149</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>17</v>
@@ -3814,7 +3814,7 @@
         <v>181</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>75</v>
@@ -3860,16 +3860,16 @@
     <row r="59" spans="1:26" ht="15" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C59" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="D59" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="E59" s="13" t="s">
         <v>190</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>191</v>
       </c>
       <c r="F59" s="17">
         <v>9.49</v>
@@ -4647,10 +4647,10 @@
         <v>108</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>110</v>
@@ -4745,31 +4745,31 @@
         <v>114</v>
       </c>
       <c r="C77" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="D77" s="13" t="s">
-        <v>186</v>
-      </c>
       <c r="E77" s="12" t="s">
-        <v>192</v>
+        <v>236</v>
       </c>
       <c r="F77" s="17">
-        <v>305</v>
+        <v>355</v>
       </c>
       <c r="G77" s="17">
         <f t="shared" si="7"/>
-        <v>396.5</v>
+        <v>461.5</v>
       </c>
       <c r="H77" s="4">
         <v>1</v>
       </c>
       <c r="I77" s="17">
         <f t="shared" si="8"/>
-        <v>396.5</v>
+        <v>461.5</v>
       </c>
       <c r="J77" s="16">
         <f t="shared" si="9"/>
-        <v>305</v>
+        <v>355</v>
       </c>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
@@ -5094,11 +5094,11 @@
       </c>
       <c r="I85" s="36">
         <f>SUM($I58:$I$81)</f>
-        <v>2645.9240000000004</v>
+        <v>2710.9240000000004</v>
       </c>
       <c r="J85" s="37">
         <f>I85/1.3</f>
-        <v>2035.3261538461541</v>
+        <v>2085.3261538461543</v>
       </c>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
@@ -5190,15 +5190,15 @@
       <c r="F88" s="17"/>
       <c r="G88" s="17"/>
       <c r="H88" s="34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I88" s="16">
         <f>SUM(I83:I86)</f>
-        <v>8873.4668000000001</v>
+        <v>8938.4668000000001</v>
       </c>
       <c r="J88" s="16">
         <f>SUM(J83:J86)</f>
-        <v>6825.743692307693</v>
+        <v>6875.743692307693</v>
       </c>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
@@ -5227,10 +5227,10 @@
       <c r="G89" s="17"/>
       <c r="H89" s="1"/>
       <c r="I89" s="38" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J89" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>

</xml_diff>